<commit_message>
Add screenshot capture on failure and fix modal link locators
- Implement Base64 screenshot embedding in ExtentReport for failed tests
- Fix successful/errored transaction link selectors to use button[1]
- Add explicit waits and filtering for clickable elements
- Enable headless mode for CI/CD compatibility
</commit_message>
<xml_diff>
--- a/src/test/resources/testcases/testcases.xlsx
+++ b/src/test/resources/testcases/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.prakash\.gemini\antigravity\scratch\transaction-insights-automation\src\test\resources\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5D4EE6-81ED-41B8-877D-1B6E59B8558F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B981DE-7A84-455E-84AB-D2AB050C1BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Application is running</t>
   </si>
   <si>
-    <t>1. Navigate to http://localhost:3001/</t>
-  </si>
-  <si>
     <t>1. Dashboard loads.
 2. 'Transaction Insights Dashboard' title is visible.
 3. Transaction table is displayed with data.</t>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>1. A dropdown menu appears (e.g., View Details, Download). *Note: Feature availability to be confirmed.*</t>
+  </si>
+  <si>
+    <t>1. Navigate to http://localhost:3000/</t>
   </si>
 </sst>
 </file>
@@ -579,11 +579,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -616,10 +622,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -627,19 +633,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -647,19 +653,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -667,19 +673,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -687,19 +693,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>
@@ -707,19 +713,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -727,19 +733,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
       </c>
       <c r="F8" t="s">
         <v>0</v>
@@ -747,19 +753,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -767,19 +773,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
       </c>
       <c r="F10" t="s">
         <v>0</v>
@@ -787,19 +793,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
@@ -807,19 +813,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>53</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
       </c>
       <c r="F12" t="s">
         <v>0</v>
@@ -827,19 +833,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>57</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
@@ -847,19 +853,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
         <v>59</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>62</v>
       </c>
       <c r="F14" t="s">
         <v>0</v>

</xml_diff>